<commit_message>
v2 Gantt extended to March 2018
</commit_message>
<xml_diff>
--- a/Laurence Gannt Plan.xlsx
+++ b/Laurence Gannt Plan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helgr\thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Submission</t>
   </si>
   <si>
-    <t>Potential Further Applications Chapter</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -243,12 +240,30 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Meas. for Option 015 MUF Paper</t>
+  </si>
+  <si>
+    <t>Write Option 015 MUF Paper</t>
+  </si>
+  <si>
+    <t>Develop MUF &gt; Opt 015 for Haris Paper</t>
+  </si>
+  <si>
+    <t>Meas. for Potential Mixer Paper</t>
+  </si>
+  <si>
+    <t>Write Potential Mixer Paper</t>
+  </si>
+  <si>
+    <t>Contingency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,18 +365,18 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -408,7 +423,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -554,7 +569,7 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -623,54 +638,54 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="19" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="9" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -679,8 +694,8 @@
     <cellStyle name="Activity" xfId="2"/>
     <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
     <cellStyle name="Actual legend" xfId="15"/>
-    <cellStyle name="Bad" xfId="19" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="19" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
@@ -695,7 +710,233 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1082,10 +1323,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AP20"/>
+  <dimension ref="B1:AP25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1111,13 +1352,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:42" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1125,102 +1366,102 @@
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="33"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="28" t="s">
+      <c r="V2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="35"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="38"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="19"/>
-      <c r="AI2" s="28" t="s">
+      <c r="AI2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
-      <c r="AO2" s="29"/>
-      <c r="AP2" s="29"/>
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
     </row>
     <row r="3" spans="2:42" s="11" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27" t="s">
+      <c r="I3" s="25"/>
+      <c r="J3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27" t="s">
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27" t="s">
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27" t="s">
+      <c r="W3" s="25"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="26" t="s">
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="26"/>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="26" t="s">
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="26"/>
-      <c r="AK3" s="26"/>
-      <c r="AL3" s="26" t="s">
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="AM3" s="26"/>
-      <c r="AN3" s="26"/>
-      <c r="AO3" s="26"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AO3" s="37"/>
     </row>
     <row r="4" spans="2:42" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4"/>
@@ -1253,22 +1494,22 @@
       <c r="AA4" s="10"/>
     </row>
     <row r="5" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="3">
@@ -1378,8 +1619,8 @@
       </c>
     </row>
     <row r="6" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
-        <v>14</v>
+      <c r="B6" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1396,16 +1637,14 @@
       <c r="G6" s="8">
         <v>0</v>
       </c>
-      <c r="M6" s="23" t="s">
-        <v>39</v>
-      </c>
+      <c r="M6" s="38"/>
     </row>
     <row r="7" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
-        <v>29</v>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="7">
         <v>2</v>
@@ -1419,13 +1658,13 @@
       <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="M7" s="23" t="s">
-        <v>42</v>
+      <c r="M7" s="38" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C8" s="7">
         <v>3</v>
@@ -1442,39 +1681,39 @@
       <c r="G8" s="8">
         <v>0</v>
       </c>
-      <c r="M8" s="23" t="s">
-        <v>42</v>
+      <c r="M8" s="38" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="M9" s="38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7">
-        <v>2</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
-        <v>30</v>
-      </c>
       <c r="C10" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" s="7">
         <v>2</v>
@@ -1488,87 +1727,87 @@
       <c r="G10" s="8">
         <v>0</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="M11" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="7">
+        <v>7</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="7">
-        <v>5</v>
-      </c>
-      <c r="D11" s="7">
+    <row r="13" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="7">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="38"/>
+    </row>
+    <row r="14" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="7">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7">
         <v>1</v>
       </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="7">
-        <v>5</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="M12" s="23"/>
-    </row>
-    <row r="13" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="7">
-        <v>5</v>
-      </c>
-      <c r="D13" s="7">
-        <v>3</v>
-      </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="M13" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="7">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7">
-        <v>2</v>
-      </c>
       <c r="E14" s="7">
         <v>0</v>
       </c>
@@ -1578,16 +1817,16 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-      <c r="M14" s="23" t="s">
-        <v>41</v>
+      <c r="M14" s="38" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
-        <v>32</v>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="7">
         <v>2</v>
@@ -1601,66 +1840,62 @@
       <c r="G15" s="8">
         <v>0</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="38"/>
+    </row>
+    <row r="16" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7">
+        <v>9</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="M16" s="38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="9">
-        <v>10</v>
-      </c>
-      <c r="D16" s="7">
+    <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="7">
+        <v>13</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="M17" s="38"/>
+    </row>
+    <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="7">
+        <v>13</v>
+      </c>
+      <c r="D18" s="7">
         <v>2</v>
       </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="M16" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="7">
-        <v>12</v>
-      </c>
-      <c r="D17" s="7">
-        <v>2</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="8">
-        <v>0</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="7">
-        <v>14</v>
-      </c>
-      <c r="D18" s="7">
-        <v>3</v>
-      </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
@@ -1668,51 +1903,164 @@
         <v>0</v>
       </c>
       <c r="G18" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="M18" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="38"/>
     </row>
     <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="7">
+        <v>13</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+      <c r="M19" s="38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="7">
+        <v>17</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="M20" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="9">
+        <v>21</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+      <c r="M21" s="38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7">
+        <v>25</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="M22" s="38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="7">
+        <v>27</v>
+      </c>
+      <c r="D23" s="7">
+        <v>3</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0</v>
+      </c>
+      <c r="M23" s="38"/>
+    </row>
+    <row r="24" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="7">
-        <v>17</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C24" s="7">
+        <v>30</v>
+      </c>
+      <c r="D24" s="7">
         <v>1</v>
       </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>0</v>
-      </c>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="7">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-      <c r="M20" s="23"/>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+      <c r="M24" s="38"/>
+    </row>
+    <row r="25" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="7">
+        <v>30</v>
+      </c>
+      <c r="D25" s="7">
+        <v>5</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+      <c r="M25" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1732,40 +2080,92 @@
     <mergeCell ref="AD3:AG3"/>
     <mergeCell ref="AH3:AK3"/>
   </mergeCells>
-  <conditionalFormatting sqref="H6:L20 N6:AP20">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="H6:L7 N6:AP7 N16:AP25 H16:L25 N9:AP13 H9:L13">
+    <cfRule type="expression" dxfId="25" priority="17">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="24" priority="19">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="23" priority="20">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="22" priority="21">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>H$5=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="19" priority="27">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="18" priority="28">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:BO21">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B26:BO26">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:AP5">
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>H$5=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:L15 N14:AP15">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>H$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:L8 N8:AP8">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>H$5=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>H$5=period_selected</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">

</xml_diff>